<commit_message>
Sofa: all tests (88) pass
</commit_message>
<xml_diff>
--- a/AstroLib.Core/SOFA/Dll Import Signatures.xlsx
+++ b/AstroLib.Core/SOFA/Dll Import Signatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevCS\AstroLib\AstroLib.Core\SOFA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07EAE74-BF46-44D7-96D3-365F92B0F985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E2C37E-1D2D-420B-AD3A-CCAC211A93CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20175" yWindow="4995" windowWidth="17370" windowHeight="13785" xr2:uid="{2686E140-CD91-4597-9EAB-8596817F2E05}"/>
+    <workbookView xWindow="-19455" yWindow="3390" windowWidth="17370" windowHeight="13785" xr2:uid="{2686E140-CD91-4597-9EAB-8596817F2E05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>in SOFA signature:</t>
   </si>
@@ -207,6 +207,22 @@
   </si>
   <si>
     <t>double[,] x</t>
+  </si>
+  <si>
+    <t>char ch[2] // RETURNED</t>
+  </si>
+  <si>
+    <t>A2tf</t>
+  </si>
+  <si>
+    <t>[In, Out] char[] signChar,</t>
+  </si>
+  <si>
+    <t>char[] signChar = {'X'}; [before call]
+string str = new string(signChar); [after]</t>
+  </si>
+  <si>
+    <t>returns string</t>
   </si>
 </sst>
 </file>
@@ -611,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B8B5D-6865-470C-ADF8-657939E71521}">
-  <dimension ref="A4:E19"/>
+  <dimension ref="A4:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -813,44 +829,61 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="8"/>
+    <row r="17" spans="1:5" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>